<commit_message>
docstring edits and tests
</commit_message>
<xml_diff>
--- a/input/example_masterfile.xlsx
+++ b/input/example_masterfile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katiebuntic/projects/RRED/rred-reports/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AAAFF2-EA41-FE4B-A4B3-34744926D4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D28A3F4-7B6D-C74B-8CB0-BDC9DEE5440A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2032" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="214">
   <si>
     <t>reg_rr_title</t>
   </si>
@@ -681,9 +681,6 @@
   </si>
   <si>
     <t>test_4_2021-22</t>
-  </si>
-  <si>
-    <t>/Users/katiebuntic/projects/RRED/rred-reports/output/reports/RRS2030220.docx</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1056,7 @@
   <dimension ref="A1:BR36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1930,7 +1927,9 @@
       <c r="F5" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>197</v>
+      </c>
       <c r="H5" t="s">
         <v>69</v>
       </c>
@@ -2093,17 +2092,17 @@
       <c r="BI5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BJ5" s="2" t="s">
-        <v>69</v>
+      <c r="BJ5" s="2">
+        <v>43443</v>
       </c>
       <c r="BK5" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="BL5" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="BM5" s="1" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="BN5" t="s">
         <v>69</v>
@@ -2398,7 +2397,7 @@
         <v>69</v>
       </c>
       <c r="X7" t="s">
-        <v>214</v>
+        <v>69</v>
       </c>
       <c r="Y7" t="s">
         <v>69</v>
@@ -2511,17 +2510,17 @@
       <c r="BI7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BJ7" s="2" t="s">
-        <v>69</v>
+      <c r="BJ7" s="2">
+        <v>44539</v>
       </c>
       <c r="BK7" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="BL7" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="BM7" s="1" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
       <c r="BN7" t="s">
         <v>69</v>

</xml_diff>